<commit_message>
Change accepted status string from 'accepted' to 'accept'.
</commit_message>
<xml_diff>
--- a/meta/objects/CommonResponse.xlsx
+++ b/meta/objects/CommonResponse.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="valueObject" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Submit有無" localSheetId="0">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
@@ -105,11 +102,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>応答ステータス．通信上のエラーとvalidationエラーの場合は"dismiss"を，&lt;br&gt;
-業務ロジックまで処理が到達した場合は"accepted"を返す</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>errors</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -243,6 +235,11 @@
   </si>
   <si>
     <t>共通レスポンスを表すオブジェクトです。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>応答ステータス．通信上のエラーとvalidationエラーの場合は"dismiss"を，&lt;br&gt;
+業務ロジックまで処理が到達した場合は"accept"を返す</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -835,51 +832,51 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -960,19 +957,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="valueObject"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1302,8 +1286,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1320,25 +1304,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1366,16 +1350,16 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="44"/>
+      <c r="K6" s="39"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="11"/>
@@ -1384,7 +1368,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="44"/>
+      <c r="K7" s="39"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
@@ -1393,16 +1377,16 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="45"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="38"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="44"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
@@ -1411,7 +1395,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -1431,7 +1415,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -1462,7 +1446,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
@@ -1517,7 +1501,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1536,67 +1520,67 @@
       <c r="P15" s="14"/>
     </row>
     <row r="16" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="47" t="s">
         <v>33</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>34</v>
       </c>
       <c r="H16" s="48"/>
       <c r="I16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="48"/>
+      <c r="K16" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" s="39" t="s">
+      <c r="L16" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="39"/>
+      <c r="M16" s="49"/>
       <c r="N16" s="15"/>
       <c r="O16" s="16"/>
       <c r="P16" s="9"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="51" t="s">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="51" t="s">
+      <c r="I17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="51" t="s">
+      <c r="J17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="K17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
       <c r="N17" s="17"/>
       <c r="O17" s="29"/>
       <c r="P17" s="14"/>
@@ -1614,11 +1598,11 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="54"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
       <c r="L18" s="20" t="s">
         <v>12</v>
       </c>
@@ -1645,12 +1629,12 @@
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
-      <c r="L19" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
+      <c r="L19" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
@@ -1658,13 +1642,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1674,7 +1658,7 @@
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -1686,10 +1670,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>21</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -1700,7 +1684,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
@@ -1713,12 +1697,12 @@
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
       <c r="L22" s="20"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
@@ -1749,12 +1733,12 @@
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
       <c r="L24" s="20"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
@@ -1785,12 +1769,12 @@
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
       <c r="L26" s="20"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>

</xml_diff>